<commit_message>
edit umkm.xlsx dan RUMAH KOS DAN TOKO JAMU.xlsx tambah field rt rw
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/DATA DATA YANG HARUS DIMASUKAN/EKONOMI/RUMAH KOS DAN TOKO JAMU.xlsx
+++ b/DOKUMEN  PENDUKUNG/DATA DATA YANG HARUS DIMASUKAN/EKONOMI/RUMAH KOS DAN TOKO JAMU.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sipepeng\DOKUMEN  PENDUKUNG\DATA DATA YANG HARUS DIMASUKAN\EKONOMI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="14235" windowHeight="6915"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="198">
   <si>
     <t>NO</t>
   </si>
@@ -601,6 +606,15 @@
   </si>
   <si>
     <t>rekapitulasi /rw saja</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>09</t>
   </si>
 </sst>
 </file>
@@ -669,7 +683,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -800,11 +814,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -878,6 +905,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -893,7 +927,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,6 +941,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -951,7 +992,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -986,7 +1027,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1195,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="X107" sqref="X107"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,72 +1247,78 @@
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1280,8 +1327,9 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>0</v>
       </c>
@@ -1291,23 +1339,26 @@
       <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -1317,19 +1368,22 @@
       <c r="C8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="13">
         <v>6</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="20">
+      <c r="G8" s="13"/>
+      <c r="H8" s="20">
         <v>2400000</v>
       </c>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1339,19 +1393,22 @@
       <c r="C9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="13">
         <v>3</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="20">
+      <c r="G9" s="13"/>
+      <c r="H9" s="20">
         <v>6000000</v>
       </c>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -1361,19 +1418,22 @@
       <c r="C10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="19">
+        <v>14</v>
+      </c>
+      <c r="E10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="20">
+      <c r="G10" s="13"/>
+      <c r="H10" s="20">
         <v>1050000</v>
       </c>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
@@ -1383,19 +1443,22 @@
       <c r="C11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="19">
+        <v>14</v>
+      </c>
+      <c r="E11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="20">
+      <c r="G11" s="13"/>
+      <c r="H11" s="20">
         <v>1050000</v>
       </c>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
@@ -1405,19 +1468,22 @@
       <c r="C12" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="19">
+        <v>14</v>
+      </c>
+      <c r="E12" s="13">
         <v>10</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="20">
+      <c r="G12" s="13"/>
+      <c r="H12" s="20">
         <v>900000</v>
       </c>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -1427,19 +1493,22 @@
       <c r="C13" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="19">
+        <v>14</v>
+      </c>
+      <c r="E13" s="13">
         <v>4</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="20">
+      <c r="G13" s="13"/>
+      <c r="H13" s="20">
         <v>1200000</v>
       </c>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>37</v>
       </c>
@@ -1449,19 +1518,22 @@
       <c r="C14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="19">
+        <v>14</v>
+      </c>
+      <c r="E14" s="13">
         <v>4</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="F14" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="20">
+      <c r="G14" s="13"/>
+      <c r="H14" s="20">
         <v>900000</v>
       </c>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
@@ -1471,19 +1543,22 @@
       <c r="C15" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="19">
+        <v>11</v>
+      </c>
+      <c r="E15" s="13">
         <v>4</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="12">
+      <c r="F15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="12">
         <v>3600000</v>
       </c>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>9</v>
       </c>
@@ -1493,19 +1568,22 @@
       <c r="C16" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="19">
+        <v>11</v>
+      </c>
+      <c r="E16" s="13">
         <v>19</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="12">
+      <c r="F16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="12">
         <v>4800000</v>
       </c>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>10</v>
       </c>
@@ -1515,19 +1593,20 @@
       <c r="C17" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="19"/>
+      <c r="E17" s="13">
         <v>38</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="12">
+      <c r="F17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="12">
         <v>3600000</v>
       </c>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>11</v>
       </c>
@@ -1537,19 +1616,20 @@
       <c r="C18" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="19"/>
+      <c r="E18" s="13">
         <v>8</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="12">
+      <c r="F18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="12">
         <v>4800000</v>
       </c>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="22">
         <v>12</v>
       </c>
@@ -1559,19 +1639,22 @@
       <c r="C19" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="25">
         <v>10</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="27">
+      <c r="F19" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27">
         <v>4800000</v>
       </c>
-      <c r="H19" s="26"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="26"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>13</v>
       </c>
@@ -1581,19 +1664,22 @@
       <c r="C20" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" s="13">
         <v>4</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="12">
+      <c r="F20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="12">
         <v>4200000</v>
       </c>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>14</v>
       </c>
@@ -1603,19 +1689,22 @@
       <c r="C21" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E21" s="13">
         <v>7</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="12">
+      <c r="F21" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="12">
         <v>3000000</v>
       </c>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>15</v>
       </c>
@@ -1625,19 +1714,22 @@
       <c r="C22" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E22" s="13">
         <v>18</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="12">
+      <c r="F22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="12">
         <v>3600000</v>
       </c>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>16</v>
       </c>
@@ -1647,19 +1739,22 @@
       <c r="C23" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" s="13">
         <v>12</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="12">
+      <c r="F23" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="12">
         <v>2600000</v>
       </c>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>17</v>
       </c>
@@ -1669,19 +1764,22 @@
       <c r="C24" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E24" s="13">
         <v>1</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="12">
+      <c r="F24" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="12">
         <v>2600000</v>
       </c>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>18</v>
       </c>
@@ -1691,19 +1789,22 @@
       <c r="C25" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E25" s="13">
         <v>10</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="12">
+      <c r="F25" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="12">
         <v>2600000</v>
       </c>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>19</v>
       </c>
@@ -1713,19 +1814,22 @@
       <c r="C26" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E26" s="13">
         <v>20</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="12">
+      <c r="F26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="12">
         <v>2600000</v>
       </c>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>20</v>
       </c>
@@ -1735,19 +1839,22 @@
       <c r="C27" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E27" s="13">
         <v>16</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="12">
+      <c r="F27" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="12">
         <v>2600000</v>
       </c>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>21</v>
       </c>
@@ -1757,19 +1864,22 @@
       <c r="C28" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E28" s="13">
         <v>7</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="12">
+      <c r="F28" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="12">
         <v>2600000</v>
       </c>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>22</v>
       </c>
@@ -1779,19 +1889,22 @@
       <c r="C29" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E29" s="13">
         <v>11</v>
       </c>
-      <c r="E29" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="12">
+      <c r="F29" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="12">
         <v>2600000</v>
       </c>
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>23</v>
       </c>
@@ -1801,19 +1914,22 @@
       <c r="C30" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E30" s="13">
         <v>3</v>
       </c>
-      <c r="E30" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="12">
+      <c r="F30" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="12">
         <v>2600000</v>
       </c>
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>24</v>
       </c>
@@ -1823,19 +1939,22 @@
       <c r="C31" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="13">
         <v>4</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="12">
+      <c r="F31" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="H31" s="12">
         <v>2600000</v>
       </c>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>25</v>
       </c>
@@ -1845,19 +1964,22 @@
       <c r="C32" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E32" s="13">
         <v>2</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="12">
+      <c r="F32" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="12">
         <v>2600000</v>
       </c>
-      <c r="H32" s="9"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>26</v>
       </c>
@@ -1867,19 +1989,22 @@
       <c r="C33" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E33" s="13">
         <v>2</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="12">
+      <c r="F33" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="12">
         <v>2600000</v>
       </c>
-      <c r="H33" s="9"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>27</v>
       </c>
@@ -1889,19 +2014,22 @@
       <c r="C34" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E34" s="13">
         <v>10</v>
       </c>
-      <c r="E34" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="12">
+      <c r="F34" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="12">
         <v>2600000</v>
       </c>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>28</v>
       </c>
@@ -1911,19 +2039,22 @@
       <c r="C35" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E35" s="13">
         <v>2</v>
       </c>
-      <c r="E35" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="12">
+      <c r="F35" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G35" s="9"/>
+      <c r="H35" s="12">
         <v>2600000</v>
       </c>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>29</v>
       </c>
@@ -1933,19 +2064,20 @@
       <c r="C36" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="9"/>
+      <c r="E36" s="13">
         <v>10</v>
       </c>
-      <c r="E36" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F36" s="9"/>
-      <c r="G36" s="12">
+      <c r="F36" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="12">
         <v>4200000</v>
       </c>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>30</v>
       </c>
@@ -1955,19 +2087,20 @@
       <c r="C37" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="9"/>
+      <c r="E37" s="13">
         <v>5</v>
       </c>
-      <c r="E37" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="12">
+      <c r="F37" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37" s="12">
         <v>4200000</v>
       </c>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>31</v>
       </c>
@@ -1977,19 +2110,20 @@
       <c r="C38" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="9"/>
+      <c r="E38" s="13">
         <v>4</v>
       </c>
-      <c r="E38" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="12">
+      <c r="F38" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" s="9"/>
+      <c r="H38" s="12">
         <v>4200000</v>
       </c>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>32</v>
       </c>
@@ -1999,19 +2133,20 @@
       <c r="C39" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="9"/>
+      <c r="E39" s="13">
         <v>2</v>
       </c>
-      <c r="E39" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="12">
+      <c r="F39" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G39" s="9"/>
+      <c r="H39" s="12">
         <v>4200000</v>
       </c>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>33</v>
       </c>
@@ -2021,19 +2156,20 @@
       <c r="C40" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40" s="9"/>
+      <c r="E40" s="13">
         <v>3</v>
       </c>
-      <c r="E40" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" s="9"/>
-      <c r="G40" s="12">
+      <c r="F40" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" s="9"/>
+      <c r="H40" s="12">
         <v>4200000</v>
       </c>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>34</v>
       </c>
@@ -2043,19 +2179,20 @@
       <c r="C41" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="9"/>
+      <c r="E41" s="13">
         <v>3</v>
       </c>
-      <c r="E41" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="9"/>
-      <c r="G41" s="12">
+      <c r="F41" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G41" s="9"/>
+      <c r="H41" s="12">
         <v>4200000</v>
       </c>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>35</v>
       </c>
@@ -2065,19 +2202,20 @@
       <c r="C42" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="13">
+      <c r="D42" s="9"/>
+      <c r="E42" s="13">
         <v>2</v>
       </c>
-      <c r="E42" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="12">
+      <c r="F42" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G42" s="9"/>
+      <c r="H42" s="12">
         <v>4200000</v>
       </c>
-      <c r="H42" s="9"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>36</v>
       </c>
@@ -2087,19 +2225,20 @@
       <c r="C43" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="13">
+      <c r="D43" s="9"/>
+      <c r="E43" s="13">
         <v>9</v>
       </c>
-      <c r="E43" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="12">
+      <c r="F43" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G43" s="9"/>
+      <c r="H43" s="12">
         <v>1800000</v>
       </c>
-      <c r="H43" s="9"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>37</v>
       </c>
@@ -2109,19 +2248,20 @@
       <c r="C44" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="13">
+      <c r="D44" s="9"/>
+      <c r="E44" s="13">
         <v>5</v>
       </c>
-      <c r="E44" s="13" t="s">
+      <c r="F44" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="12">
+      <c r="G44" s="9"/>
+      <c r="H44" s="12">
         <v>2040000</v>
       </c>
-      <c r="H44" s="9"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>38</v>
       </c>
@@ -2131,19 +2271,20 @@
       <c r="C45" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="13">
+      <c r="D45" s="9"/>
+      <c r="E45" s="13">
         <v>1</v>
       </c>
-      <c r="E45" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" s="9"/>
-      <c r="G45" s="12">
+      <c r="F45" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G45" s="9"/>
+      <c r="H45" s="12">
         <v>1440000</v>
       </c>
-      <c r="H45" s="9"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>39</v>
       </c>
@@ -2153,19 +2294,20 @@
       <c r="C46" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D46" s="13">
+      <c r="D46" s="9"/>
+      <c r="E46" s="13">
         <v>2</v>
       </c>
-      <c r="E46" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" s="9"/>
-      <c r="G46" s="12">
+      <c r="F46" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G46" s="9"/>
+      <c r="H46" s="12">
         <v>1440000</v>
       </c>
-      <c r="H46" s="9"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>40</v>
       </c>
@@ -2175,19 +2317,20 @@
       <c r="C47" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="13">
+      <c r="D47" s="9"/>
+      <c r="E47" s="13">
         <v>1</v>
       </c>
-      <c r="E47" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" s="9"/>
-      <c r="G47" s="12">
+      <c r="F47" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G47" s="9"/>
+      <c r="H47" s="12">
         <v>1440000</v>
       </c>
-      <c r="H47" s="9"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>41</v>
       </c>
@@ -2197,19 +2340,20 @@
       <c r="C48" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="13">
+      <c r="D48" s="9"/>
+      <c r="E48" s="13">
         <v>1</v>
       </c>
-      <c r="E48" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" s="9"/>
-      <c r="G48" s="12">
+      <c r="F48" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G48" s="9"/>
+      <c r="H48" s="12">
         <v>1440000</v>
       </c>
-      <c r="H48" s="9"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>42</v>
       </c>
@@ -2219,19 +2363,20 @@
       <c r="C49" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D49" s="13">
+      <c r="D49" s="9"/>
+      <c r="E49" s="13">
         <v>4</v>
       </c>
-      <c r="E49" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F49" s="9"/>
-      <c r="G49" s="12">
+      <c r="F49" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G49" s="9"/>
+      <c r="H49" s="12">
         <v>1440000</v>
       </c>
-      <c r="H49" s="9"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>43</v>
       </c>
@@ -2241,19 +2386,20 @@
       <c r="C50" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="13">
+      <c r="D50" s="9"/>
+      <c r="E50" s="13">
         <v>8</v>
       </c>
-      <c r="E50" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F50" s="9"/>
-      <c r="G50" s="12">
+      <c r="F50" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G50" s="9"/>
+      <c r="H50" s="12">
         <v>1440000</v>
       </c>
-      <c r="H50" s="9"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>44</v>
       </c>
@@ -2263,19 +2409,20 @@
       <c r="C51" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D51" s="13">
+      <c r="D51" s="9"/>
+      <c r="E51" s="13">
         <v>3</v>
       </c>
-      <c r="E51" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="12">
+      <c r="F51" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G51" s="9"/>
+      <c r="H51" s="12">
         <v>1200000</v>
       </c>
-      <c r="H51" s="9"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>45</v>
       </c>
@@ -2285,19 +2432,20 @@
       <c r="C52" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D52" s="13">
+      <c r="D52" s="9"/>
+      <c r="E52" s="13">
         <v>4</v>
       </c>
-      <c r="E52" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F52" s="9"/>
-      <c r="G52" s="12">
+      <c r="F52" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G52" s="9"/>
+      <c r="H52" s="12">
         <v>3000000</v>
       </c>
-      <c r="H52" s="9"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>46</v>
       </c>
@@ -2307,19 +2455,20 @@
       <c r="C53" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D53" s="13">
+      <c r="D53" s="9"/>
+      <c r="E53" s="13">
         <v>10</v>
       </c>
-      <c r="E53" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F53" s="9"/>
-      <c r="G53" s="12">
+      <c r="F53" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G53" s="9"/>
+      <c r="H53" s="12">
         <v>2400000</v>
       </c>
-      <c r="H53" s="9"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>47</v>
       </c>
@@ -2329,19 +2478,20 @@
       <c r="C54" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="13">
+      <c r="D54" s="9"/>
+      <c r="E54" s="13">
         <v>3</v>
       </c>
-      <c r="E54" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F54" s="9"/>
-      <c r="G54" s="12">
+      <c r="F54" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G54" s="9"/>
+      <c r="H54" s="12">
         <v>2400000</v>
       </c>
-      <c r="H54" s="9"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>48</v>
       </c>
@@ -2351,19 +2501,20 @@
       <c r="C55" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D55" s="13">
+      <c r="D55" s="9"/>
+      <c r="E55" s="13">
         <v>4</v>
       </c>
-      <c r="E55" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F55" s="9"/>
-      <c r="G55" s="12">
+      <c r="F55" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G55" s="9"/>
+      <c r="H55" s="12">
         <v>2400000</v>
       </c>
-      <c r="H55" s="9"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>49</v>
       </c>
@@ -2373,19 +2524,20 @@
       <c r="C56" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D56" s="13">
+      <c r="D56" s="9"/>
+      <c r="E56" s="13">
         <v>10</v>
       </c>
-      <c r="E56" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F56" s="9"/>
-      <c r="G56" s="12">
+      <c r="F56" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G56" s="9"/>
+      <c r="H56" s="12">
         <v>2400000</v>
       </c>
-      <c r="H56" s="9"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>50</v>
       </c>
@@ -2395,19 +2547,20 @@
       <c r="C57" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D57" s="13">
+      <c r="D57" s="9"/>
+      <c r="E57" s="13">
         <v>9</v>
       </c>
-      <c r="E57" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F57" s="9"/>
-      <c r="G57" s="12">
+      <c r="F57" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G57" s="9"/>
+      <c r="H57" s="12">
         <v>2400000</v>
       </c>
-      <c r="H57" s="9"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="9"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>51</v>
       </c>
@@ -2417,19 +2570,20 @@
       <c r="C58" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D58" s="13">
+      <c r="D58" s="9"/>
+      <c r="E58" s="13">
         <v>8</v>
       </c>
-      <c r="E58" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F58" s="9"/>
-      <c r="G58" s="12">
+      <c r="F58" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G58" s="9"/>
+      <c r="H58" s="12">
         <v>2400000</v>
       </c>
-      <c r="H58" s="9"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="9"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>52</v>
       </c>
@@ -2439,19 +2593,20 @@
       <c r="C59" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D59" s="13">
+      <c r="D59" s="9"/>
+      <c r="E59" s="13">
         <v>16</v>
       </c>
-      <c r="E59" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F59" s="9"/>
-      <c r="G59" s="12">
+      <c r="F59" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G59" s="9"/>
+      <c r="H59" s="12">
         <v>4800000</v>
       </c>
-      <c r="H59" s="9"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="9"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>53</v>
       </c>
@@ -2461,19 +2616,20 @@
       <c r="C60" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="13">
+      <c r="D60" s="9"/>
+      <c r="E60" s="13">
         <v>10</v>
       </c>
-      <c r="E60" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F60" s="9"/>
-      <c r="G60" s="12">
+      <c r="F60" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G60" s="9"/>
+      <c r="H60" s="12">
         <v>4800000</v>
       </c>
-      <c r="H60" s="9"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="9"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>54</v>
       </c>
@@ -2483,19 +2639,20 @@
       <c r="C61" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D61" s="13">
+      <c r="D61" s="9"/>
+      <c r="E61" s="13">
         <v>6</v>
       </c>
-      <c r="E61" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F61" s="9"/>
-      <c r="G61" s="12">
+      <c r="F61" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G61" s="9"/>
+      <c r="H61" s="12">
         <v>4800000</v>
       </c>
-      <c r="H61" s="9"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="9"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>55</v>
       </c>
@@ -2505,19 +2662,20 @@
       <c r="C62" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D62" s="13">
+      <c r="D62" s="9"/>
+      <c r="E62" s="13">
         <v>8</v>
       </c>
-      <c r="E62" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F62" s="9"/>
-      <c r="G62" s="12">
+      <c r="F62" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G62" s="9"/>
+      <c r="H62" s="12">
         <v>4800000</v>
       </c>
-      <c r="H62" s="9"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="9"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>56</v>
       </c>
@@ -2527,19 +2685,20 @@
       <c r="C63" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D63" s="9"/>
+      <c r="E63" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E63" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F63" s="9"/>
-      <c r="G63" s="12">
+      <c r="F63" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G63" s="9"/>
+      <c r="H63" s="12">
         <v>4800000</v>
       </c>
-      <c r="H63" s="9"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="9"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>57</v>
       </c>
@@ -2549,19 +2708,20 @@
       <c r="C64" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="D64" s="9"/>
+      <c r="E64" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E64" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F64" s="9"/>
-      <c r="G64" s="12">
+      <c r="F64" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G64" s="9"/>
+      <c r="H64" s="12">
         <v>4000000</v>
       </c>
-      <c r="H64" s="9"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="9"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>58</v>
       </c>
@@ -2571,19 +2731,20 @@
       <c r="C65" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D65" s="13">
+      <c r="D65" s="9"/>
+      <c r="E65" s="13">
         <v>100</v>
       </c>
-      <c r="E65" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F65" s="9"/>
-      <c r="G65" s="12">
+      <c r="F65" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G65" s="9"/>
+      <c r="H65" s="12">
         <v>20000000</v>
       </c>
-      <c r="H65" s="9"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="9"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="13">
         <v>59</v>
       </c>
@@ -2593,19 +2754,20 @@
       <c r="C66" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D66" s="13">
+      <c r="D66" s="9"/>
+      <c r="E66" s="13">
         <v>10</v>
       </c>
-      <c r="E66" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F66" s="9"/>
-      <c r="G66" s="12">
+      <c r="F66" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G66" s="9"/>
+      <c r="H66" s="12">
         <v>4800000</v>
       </c>
-      <c r="H66" s="9"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="9"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
         <v>60</v>
       </c>
@@ -2615,19 +2777,20 @@
       <c r="C67" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D67" s="13">
+      <c r="D67" s="9"/>
+      <c r="E67" s="13">
         <v>10</v>
       </c>
-      <c r="E67" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F67" s="9"/>
-      <c r="G67" s="12">
+      <c r="F67" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G67" s="9"/>
+      <c r="H67" s="12">
         <v>4800000</v>
       </c>
-      <c r="H67" s="9"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="9"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>61</v>
       </c>
@@ -2637,19 +2800,20 @@
       <c r="C68" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D68" s="13">
+      <c r="D68" s="9"/>
+      <c r="E68" s="13">
         <v>6</v>
       </c>
-      <c r="E68" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F68" s="9"/>
-      <c r="G68" s="12">
+      <c r="F68" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G68" s="9"/>
+      <c r="H68" s="12">
         <v>4800000</v>
       </c>
-      <c r="H68" s="9"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="9"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>62</v>
       </c>
@@ -2659,19 +2823,20 @@
       <c r="C69" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D69" s="13">
+      <c r="D69" s="9"/>
+      <c r="E69" s="13">
         <v>6</v>
       </c>
-      <c r="E69" s="13" t="s">
+      <c r="F69" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="F69" s="9"/>
-      <c r="G69" s="12">
+      <c r="G69" s="9"/>
+      <c r="H69" s="12">
         <v>1920000</v>
       </c>
-      <c r="H69" s="9"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="9"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
         <v>63</v>
       </c>
@@ -2681,19 +2846,20 @@
       <c r="C70" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D70" s="13">
+      <c r="D70" s="9"/>
+      <c r="E70" s="13">
         <v>9</v>
       </c>
-      <c r="E70" s="13" t="s">
+      <c r="F70" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="F70" s="9"/>
-      <c r="G70" s="12">
+      <c r="G70" s="9"/>
+      <c r="H70" s="12">
         <v>1800000</v>
       </c>
-      <c r="H70" s="9"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="9"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
         <v>64</v>
       </c>
@@ -2703,19 +2869,20 @@
       <c r="C71" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D71" s="13">
+      <c r="D71" s="9"/>
+      <c r="E71" s="13">
         <v>6</v>
       </c>
-      <c r="E71" s="13">
+      <c r="F71" s="13">
         <v>3</v>
       </c>
-      <c r="F71" s="9"/>
-      <c r="G71" s="12">
+      <c r="G71" s="9"/>
+      <c r="H71" s="12">
         <v>3600000</v>
       </c>
-      <c r="H71" s="9"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="9"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
         <v>65</v>
       </c>
@@ -2725,19 +2892,20 @@
       <c r="C72" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D72" s="13">
-        <v>3</v>
-      </c>
+      <c r="D72" s="9"/>
       <c r="E72" s="13">
         <v>3</v>
       </c>
-      <c r="F72" s="9"/>
-      <c r="G72" s="12">
+      <c r="F72" s="13">
+        <v>3</v>
+      </c>
+      <c r="G72" s="9"/>
+      <c r="H72" s="12">
         <v>3600000</v>
       </c>
-      <c r="H72" s="9"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="9"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
         <v>66</v>
       </c>
@@ -2747,19 +2915,20 @@
       <c r="C73" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D73" s="13">
+      <c r="D73" s="9"/>
+      <c r="E73" s="13">
         <v>5</v>
       </c>
-      <c r="E73" s="13">
+      <c r="F73" s="13">
         <v>3</v>
       </c>
-      <c r="F73" s="9"/>
-      <c r="G73" s="12">
+      <c r="G73" s="9"/>
+      <c r="H73" s="12">
         <v>3600000</v>
       </c>
-      <c r="H73" s="9"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="9"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
         <v>67</v>
       </c>
@@ -2769,19 +2938,20 @@
       <c r="C74" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D74" s="13">
+      <c r="D74" s="9"/>
+      <c r="E74" s="13">
         <v>5</v>
       </c>
-      <c r="E74" s="13">
+      <c r="F74" s="13">
         <v>3</v>
       </c>
-      <c r="F74" s="9"/>
-      <c r="G74" s="12">
+      <c r="G74" s="9"/>
+      <c r="H74" s="12">
         <v>3600000</v>
       </c>
-      <c r="H74" s="9"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <v>68</v>
       </c>
@@ -2791,19 +2961,20 @@
       <c r="C75" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="D75" s="30">
+      <c r="D75" s="29"/>
+      <c r="E75" s="30">
         <v>19</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="F75" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F75" s="9"/>
-      <c r="G75" s="12">
+      <c r="G75" s="9"/>
+      <c r="H75" s="12">
         <v>3000000</v>
       </c>
-      <c r="H75" s="9"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="9"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
         <v>69</v>
       </c>
@@ -2813,19 +2984,20 @@
       <c r="C76" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="D76" s="30">
+      <c r="D76" s="29"/>
+      <c r="E76" s="30">
         <v>2</v>
       </c>
-      <c r="E76" s="30">
+      <c r="F76" s="30">
         <v>7</v>
       </c>
-      <c r="F76" s="9"/>
-      <c r="G76" s="12">
+      <c r="G76" s="9"/>
+      <c r="H76" s="12">
         <v>3500000</v>
       </c>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
         <v>70</v>
       </c>
@@ -2835,19 +3007,20 @@
       <c r="C77" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D77" s="30">
+      <c r="D77" s="29"/>
+      <c r="E77" s="30">
         <v>4</v>
       </c>
-      <c r="E77" s="30">
+      <c r="F77" s="30">
         <v>12</v>
       </c>
-      <c r="F77" s="9"/>
-      <c r="G77" s="12">
+      <c r="G77" s="9"/>
+      <c r="H77" s="12">
         <v>5000000</v>
       </c>
-      <c r="H77" s="9"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <v>71</v>
       </c>
@@ -2857,19 +3030,20 @@
       <c r="C78" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="D78" s="30">
+      <c r="D78" s="29"/>
+      <c r="E78" s="30">
         <v>3</v>
       </c>
-      <c r="E78" s="30">
+      <c r="F78" s="30">
         <v>13</v>
       </c>
-      <c r="F78" s="9"/>
-      <c r="G78" s="12">
+      <c r="G78" s="9"/>
+      <c r="H78" s="12">
         <v>8000000</v>
       </c>
-      <c r="H78" s="9"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="9"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
         <v>72</v>
       </c>
@@ -2879,19 +3053,20 @@
       <c r="C79" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D79" s="30">
+      <c r="D79" s="29"/>
+      <c r="E79" s="30">
         <v>3</v>
       </c>
-      <c r="E79" s="30">
+      <c r="F79" s="30">
         <v>7</v>
       </c>
-      <c r="F79" s="9"/>
-      <c r="G79" s="12">
+      <c r="G79" s="9"/>
+      <c r="H79" s="12">
         <v>2800000</v>
       </c>
-      <c r="H79" s="9"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="9"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
         <v>73</v>
       </c>
@@ -2901,19 +3076,20 @@
       <c r="C80" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="D80" s="30">
+      <c r="D80" s="29"/>
+      <c r="E80" s="30">
         <v>3</v>
       </c>
-      <c r="E80" s="30">
+      <c r="F80" s="30">
         <v>9</v>
       </c>
-      <c r="F80" s="9"/>
-      <c r="G80" s="12">
+      <c r="G80" s="9"/>
+      <c r="H80" s="12">
         <v>15000000</v>
       </c>
-      <c r="H80" s="9"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="9"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
         <v>75</v>
       </c>
@@ -2923,19 +3099,20 @@
       <c r="C81" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D81" s="29"/>
+      <c r="E81" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E81" s="9" t="s">
+      <c r="F81" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F81" s="9"/>
-      <c r="G81" s="12">
+      <c r="G81" s="9"/>
+      <c r="H81" s="12">
         <v>3600000</v>
       </c>
-      <c r="H81" s="9"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="9"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <v>76</v>
       </c>
@@ -2945,19 +3122,20 @@
       <c r="C82" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D82" s="9" t="s">
+      <c r="D82" s="29"/>
+      <c r="E82" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="F82" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F82" s="9"/>
-      <c r="G82" s="12">
+      <c r="G82" s="9"/>
+      <c r="H82" s="12">
         <v>15000000</v>
       </c>
-      <c r="H82" s="9"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="9"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
         <v>77</v>
       </c>
@@ -2967,19 +3145,20 @@
       <c r="C83" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D83" s="9" t="s">
+      <c r="D83" s="29"/>
+      <c r="E83" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E83" s="9" t="s">
+      <c r="F83" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F83" s="9"/>
-      <c r="G83" s="12">
+      <c r="G83" s="9"/>
+      <c r="H83" s="12">
         <v>4000000</v>
       </c>
-      <c r="H83" s="9"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="9"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="30">
         <v>78</v>
       </c>
@@ -2989,19 +3168,20 @@
       <c r="C84" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D84" s="9" t="s">
+      <c r="D84" s="29"/>
+      <c r="E84" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E84" s="9" t="s">
+      <c r="F84" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F84" s="9"/>
-      <c r="G84" s="12">
+      <c r="G84" s="9"/>
+      <c r="H84" s="12">
         <v>4000000</v>
       </c>
-      <c r="H84" s="9"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="9"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="30">
         <v>79</v>
       </c>
@@ -3011,19 +3191,20 @@
       <c r="C85" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D85" s="9" t="s">
+      <c r="D85" s="29"/>
+      <c r="E85" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E85" s="9" t="s">
+      <c r="F85" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F85" s="9"/>
-      <c r="G85" s="12">
+      <c r="G85" s="9"/>
+      <c r="H85" s="12">
         <v>4500000</v>
       </c>
-      <c r="H85" s="9"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="9"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="30">
         <v>80</v>
       </c>
@@ -3033,19 +3214,20 @@
       <c r="C86" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D86" s="9" t="s">
+      <c r="D86" s="29"/>
+      <c r="E86" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E86" s="9" t="s">
+      <c r="F86" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F86" s="9"/>
-      <c r="G86" s="12">
+      <c r="G86" s="9"/>
+      <c r="H86" s="12">
         <v>4800000</v>
       </c>
-      <c r="H86" s="9"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="9"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="30">
         <v>81</v>
       </c>
@@ -3055,19 +3237,20 @@
       <c r="C87" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D87" s="9" t="s">
+      <c r="D87" s="29"/>
+      <c r="E87" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E87" s="9" t="s">
+      <c r="F87" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F87" s="9"/>
-      <c r="G87" s="12">
+      <c r="G87" s="9"/>
+      <c r="H87" s="12">
         <v>3000000</v>
       </c>
-      <c r="H87" s="9"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="9"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="30">
         <v>82</v>
       </c>
@@ -3077,19 +3260,20 @@
       <c r="C88" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D88" s="9" t="s">
+      <c r="D88" s="29"/>
+      <c r="E88" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E88" s="9" t="s">
+      <c r="F88" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F88" s="9"/>
-      <c r="G88" s="12">
+      <c r="G88" s="9"/>
+      <c r="H88" s="12">
         <v>3500000</v>
       </c>
-      <c r="H88" s="9"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="9"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="30">
         <v>83</v>
       </c>
@@ -3099,19 +3283,20 @@
       <c r="C89" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D89" s="9" t="s">
+      <c r="D89" s="29"/>
+      <c r="E89" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E89" s="9" t="s">
+      <c r="F89" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F89" s="9"/>
-      <c r="G89" s="12">
+      <c r="G89" s="9"/>
+      <c r="H89" s="12">
         <v>3500000</v>
       </c>
-      <c r="H89" s="9"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="9"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="30">
         <v>84</v>
       </c>
@@ -3121,19 +3306,20 @@
       <c r="C90" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D90" s="9">
+      <c r="D90" s="29"/>
+      <c r="E90" s="9">
         <v>2</v>
       </c>
-      <c r="E90" s="9">
+      <c r="F90" s="9">
         <v>8</v>
       </c>
-      <c r="F90" s="9"/>
-      <c r="G90" s="12">
+      <c r="G90" s="9"/>
+      <c r="H90" s="12">
         <v>600000</v>
       </c>
-      <c r="H90" s="9"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="9"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="30">
         <v>85</v>
       </c>
@@ -3143,19 +3329,20 @@
       <c r="C91" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D91" s="9">
+      <c r="D91" s="29"/>
+      <c r="E91" s="9">
         <v>5</v>
       </c>
-      <c r="E91" s="9">
+      <c r="F91" s="9">
         <v>10</v>
       </c>
-      <c r="F91" s="9"/>
-      <c r="G91" s="12">
+      <c r="G91" s="9"/>
+      <c r="H91" s="12">
         <v>1250000</v>
       </c>
-      <c r="H91" s="9"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="9"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="30">
         <v>86</v>
       </c>
@@ -3165,19 +3352,20 @@
       <c r="C92" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D92" s="9">
+      <c r="D92" s="29"/>
+      <c r="E92" s="9">
         <v>2</v>
       </c>
-      <c r="E92" s="9">
+      <c r="F92" s="9">
         <v>3</v>
       </c>
-      <c r="F92" s="9"/>
-      <c r="G92" s="12">
+      <c r="G92" s="9"/>
+      <c r="H92" s="12">
         <v>9640000</v>
       </c>
-      <c r="H92" s="9"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="9"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="30">
         <v>87</v>
       </c>
@@ -3187,19 +3375,20 @@
       <c r="C93" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D93" s="9">
+      <c r="D93" s="29"/>
+      <c r="E93" s="9">
         <v>3</v>
       </c>
-      <c r="E93" s="9">
+      <c r="F93" s="9">
         <v>6</v>
       </c>
-      <c r="F93" s="9"/>
-      <c r="G93" s="12">
+      <c r="G93" s="9"/>
+      <c r="H93" s="12">
         <v>21000000</v>
       </c>
-      <c r="H93" s="9"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="9"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="30">
         <v>88</v>
       </c>
@@ -3209,19 +3398,20 @@
       <c r="C94" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D94" s="9">
+      <c r="D94" s="29"/>
+      <c r="E94" s="9">
         <v>1</v>
       </c>
-      <c r="E94" s="9">
+      <c r="F94" s="9">
         <v>4</v>
       </c>
-      <c r="F94" s="9"/>
-      <c r="G94" s="12">
+      <c r="G94" s="9"/>
+      <c r="H94" s="12">
         <v>12000000</v>
       </c>
-      <c r="H94" s="9"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="9"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="30">
         <v>89</v>
       </c>
@@ -3231,19 +3421,20 @@
       <c r="C95" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D95" s="9">
+      <c r="D95" s="29"/>
+      <c r="E95" s="9">
         <v>1</v>
       </c>
-      <c r="E95" s="9">
+      <c r="F95" s="9">
         <v>5</v>
       </c>
-      <c r="F95" s="9"/>
-      <c r="G95" s="12">
+      <c r="G95" s="9"/>
+      <c r="H95" s="12">
         <v>3000000</v>
       </c>
-      <c r="H95" s="9"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="9"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="30">
         <v>90</v>
       </c>
@@ -3253,19 +3444,20 @@
       <c r="C96" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D96" s="9">
+      <c r="D96" s="29"/>
+      <c r="E96" s="9">
         <v>1</v>
       </c>
-      <c r="E96" s="9">
+      <c r="F96" s="9">
         <v>5</v>
       </c>
-      <c r="F96" s="9"/>
-      <c r="G96" s="12">
+      <c r="G96" s="9"/>
+      <c r="H96" s="12">
         <v>8000000</v>
       </c>
-      <c r="H96" s="9"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="9"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="30">
         <v>91</v>
       </c>
@@ -3275,19 +3467,20 @@
       <c r="C97" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="D97" s="9">
-        <v>4</v>
-      </c>
+      <c r="D97" s="29"/>
       <c r="E97" s="9">
         <v>4</v>
       </c>
-      <c r="F97" s="9"/>
-      <c r="G97" s="12">
+      <c r="F97" s="9">
+        <v>4</v>
+      </c>
+      <c r="G97" s="9"/>
+      <c r="H97" s="12">
         <v>3000000</v>
       </c>
-      <c r="H97" s="9"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="9"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="30">
         <v>92</v>
       </c>
@@ -3297,19 +3490,20 @@
       <c r="C98" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="D98" s="9">
+      <c r="D98" s="29"/>
+      <c r="E98" s="9">
         <v>2</v>
       </c>
-      <c r="E98" s="9">
+      <c r="F98" s="9">
         <v>4</v>
       </c>
-      <c r="F98" s="9"/>
-      <c r="G98" s="12">
+      <c r="G98" s="9"/>
+      <c r="H98" s="12">
         <v>3600000</v>
       </c>
-      <c r="H98" s="9"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="9"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="30">
         <v>93</v>
       </c>
@@ -3319,19 +3513,20 @@
       <c r="C99" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="D99" s="9">
-        <v>4</v>
-      </c>
+      <c r="D99" s="29"/>
       <c r="E99" s="9">
         <v>4</v>
       </c>
-      <c r="F99" s="9"/>
-      <c r="G99" s="12">
+      <c r="F99" s="9">
+        <v>4</v>
+      </c>
+      <c r="G99" s="9"/>
+      <c r="H99" s="12">
         <v>2400000</v>
       </c>
-      <c r="H99" s="9"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="9"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="30">
         <v>94</v>
       </c>
@@ -3341,19 +3536,20 @@
       <c r="C100" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D100" s="9">
+      <c r="D100" s="29"/>
+      <c r="E100" s="9">
         <v>3</v>
       </c>
-      <c r="E100" s="9">
+      <c r="F100" s="9">
         <v>2</v>
       </c>
-      <c r="F100" s="9"/>
-      <c r="G100" s="12">
+      <c r="G100" s="9"/>
+      <c r="H100" s="12">
         <v>3600000</v>
       </c>
-      <c r="H100" s="9"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="9"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="30">
         <v>95</v>
       </c>
@@ -3363,19 +3559,20 @@
       <c r="C101" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D101" s="9">
+      <c r="D101" s="29"/>
+      <c r="E101" s="9">
         <v>2</v>
       </c>
-      <c r="E101" s="9">
+      <c r="F101" s="9">
         <v>3</v>
       </c>
-      <c r="F101" s="9"/>
-      <c r="G101" s="12">
+      <c r="G101" s="9"/>
+      <c r="H101" s="12">
         <v>3000000</v>
       </c>
-      <c r="H101" s="9"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="9"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="30">
         <v>96</v>
       </c>
@@ -3385,19 +3582,20 @@
       <c r="C102" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D102" s="9">
-        <v>2</v>
-      </c>
+      <c r="D102" s="29"/>
       <c r="E102" s="9">
         <v>2</v>
       </c>
-      <c r="F102" s="9"/>
-      <c r="G102" s="12">
+      <c r="F102" s="9">
+        <v>2</v>
+      </c>
+      <c r="G102" s="9"/>
+      <c r="H102" s="12">
         <v>2600000</v>
       </c>
-      <c r="H102" s="9"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="9"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="30">
         <v>97</v>
       </c>
@@ -3407,19 +3605,20 @@
       <c r="C103" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D103" s="9">
-        <v>2</v>
-      </c>
+      <c r="D103" s="29"/>
       <c r="E103" s="9">
         <v>2</v>
       </c>
-      <c r="F103" s="9"/>
-      <c r="G103" s="12">
+      <c r="F103" s="9">
+        <v>2</v>
+      </c>
+      <c r="G103" s="9"/>
+      <c r="H103" s="12">
         <v>2600000</v>
       </c>
-      <c r="H103" s="9"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="9"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="30">
         <v>98</v>
       </c>
@@ -3429,19 +3628,20 @@
       <c r="C104" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D104" s="9">
+      <c r="D104" s="29"/>
+      <c r="E104" s="9">
         <v>6</v>
       </c>
-      <c r="E104" s="9">
+      <c r="F104" s="9">
         <v>2</v>
       </c>
-      <c r="F104" s="9"/>
-      <c r="G104" s="12">
+      <c r="G104" s="9"/>
+      <c r="H104" s="12">
         <v>2600000</v>
       </c>
-      <c r="H104" s="9"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="9"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="30">
         <v>99</v>
       </c>
@@ -3451,19 +3651,20 @@
       <c r="C105" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D105" s="9">
-        <v>2</v>
-      </c>
+      <c r="D105" s="29"/>
       <c r="E105" s="9">
         <v>2</v>
       </c>
-      <c r="F105" s="9"/>
-      <c r="G105" s="12">
+      <c r="F105" s="9">
+        <v>2</v>
+      </c>
+      <c r="G105" s="9"/>
+      <c r="H105" s="12">
         <v>3000000</v>
       </c>
-      <c r="H105" s="9"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="9"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="30">
         <v>100</v>
       </c>
@@ -3473,19 +3674,20 @@
       <c r="C106" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D106" s="9">
+      <c r="D106" s="29"/>
+      <c r="E106" s="9">
         <v>4</v>
       </c>
-      <c r="E106" s="9">
+      <c r="F106" s="9">
         <v>2</v>
       </c>
-      <c r="F106" s="9"/>
-      <c r="G106" s="12">
+      <c r="G106" s="9"/>
+      <c r="H106" s="12">
         <v>3000000</v>
       </c>
-      <c r="H106" s="9"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="9"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="30">
         <v>101</v>
       </c>
@@ -3495,19 +3697,20 @@
       <c r="C107" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D107" s="9">
-        <v>2</v>
-      </c>
+      <c r="D107" s="29"/>
       <c r="E107" s="9">
         <v>2</v>
       </c>
-      <c r="F107" s="9"/>
-      <c r="G107" s="12">
+      <c r="F107" s="9">
+        <v>2</v>
+      </c>
+      <c r="G107" s="9"/>
+      <c r="H107" s="12">
         <v>3000000</v>
       </c>
-      <c r="H107" s="9"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="9"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="30">
         <v>102</v>
       </c>
@@ -3517,19 +3720,20 @@
       <c r="C108" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D108" s="9">
-        <v>2</v>
-      </c>
+      <c r="D108" s="29"/>
       <c r="E108" s="9">
         <v>2</v>
       </c>
-      <c r="F108" s="9"/>
-      <c r="G108" s="12">
+      <c r="F108" s="9">
+        <v>2</v>
+      </c>
+      <c r="G108" s="9"/>
+      <c r="H108" s="12">
         <v>3000000</v>
       </c>
-      <c r="H108" s="9"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="9"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="30">
         <v>103</v>
       </c>
@@ -3539,19 +3743,20 @@
       <c r="C109" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D109" s="9">
+      <c r="D109" s="29"/>
+      <c r="E109" s="9">
         <v>6</v>
       </c>
-      <c r="E109" s="9">
+      <c r="F109" s="9">
         <v>3</v>
       </c>
-      <c r="F109" s="9"/>
-      <c r="G109" s="12">
+      <c r="G109" s="9"/>
+      <c r="H109" s="12">
         <v>4800000</v>
       </c>
-      <c r="H109" s="9"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="9"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="30">
         <v>104</v>
       </c>
@@ -3561,19 +3766,20 @@
       <c r="C110" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D110" s="9">
+      <c r="D110" s="29"/>
+      <c r="E110" s="9">
         <v>6</v>
       </c>
-      <c r="E110" s="9">
+      <c r="F110" s="9">
         <v>4</v>
       </c>
-      <c r="F110" s="9"/>
-      <c r="G110" s="12">
+      <c r="G110" s="9"/>
+      <c r="H110" s="12">
         <v>1800000</v>
       </c>
-      <c r="H110" s="9"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="9"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="30">
         <v>105</v>
       </c>
@@ -3583,19 +3789,20 @@
       <c r="C111" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D111" s="9">
-        <v>3</v>
-      </c>
+      <c r="D111" s="29"/>
       <c r="E111" s="9">
         <v>3</v>
       </c>
-      <c r="F111" s="9"/>
-      <c r="G111" s="12">
+      <c r="F111" s="9">
+        <v>3</v>
+      </c>
+      <c r="G111" s="9"/>
+      <c r="H111" s="12">
         <v>2100000</v>
       </c>
-      <c r="H111" s="9"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" s="9"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="30">
         <v>106</v>
       </c>
@@ -3605,19 +3812,20 @@
       <c r="C112" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D112" s="9">
+      <c r="D112" s="29"/>
+      <c r="E112" s="9">
         <v>1</v>
       </c>
-      <c r="E112" s="9">
+      <c r="F112" s="9">
         <v>3</v>
       </c>
-      <c r="F112" s="9"/>
-      <c r="G112" s="12">
+      <c r="G112" s="9"/>
+      <c r="H112" s="12">
         <v>5000000</v>
       </c>
-      <c r="H112" s="9"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="9"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="30">
         <v>107</v>
       </c>
@@ -3627,19 +3835,20 @@
       <c r="C113" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D113" s="9">
+      <c r="D113" s="29"/>
+      <c r="E113" s="9">
         <v>2</v>
       </c>
-      <c r="E113" s="9">
+      <c r="F113" s="9">
         <v>1</v>
       </c>
-      <c r="F113" s="9"/>
-      <c r="G113" s="12">
+      <c r="G113" s="9"/>
+      <c r="H113" s="12">
         <v>3000000</v>
       </c>
-      <c r="H113" s="9"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="9"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="30">
         <v>108</v>
       </c>
@@ -3649,19 +3858,20 @@
       <c r="C114" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D114" s="9">
+      <c r="D114" s="29"/>
+      <c r="E114" s="9">
         <v>1</v>
       </c>
-      <c r="E114" s="9">
+      <c r="F114" s="9">
         <v>3</v>
       </c>
-      <c r="F114" s="9"/>
-      <c r="G114" s="12">
+      <c r="G114" s="9"/>
+      <c r="H114" s="12">
         <v>2100000</v>
       </c>
-      <c r="H114" s="9"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" s="9"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="30">
         <v>109</v>
       </c>
@@ -3671,19 +3881,20 @@
       <c r="C115" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D115" s="9">
-        <v>2</v>
-      </c>
+      <c r="D115" s="29"/>
       <c r="E115" s="9">
         <v>2</v>
       </c>
-      <c r="F115" s="9"/>
-      <c r="G115" s="12">
+      <c r="F115" s="9">
+        <v>2</v>
+      </c>
+      <c r="G115" s="9"/>
+      <c r="H115" s="12">
         <v>3000000</v>
       </c>
-      <c r="H115" s="9"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="9"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="30">
         <v>110</v>
       </c>
@@ -3693,19 +3904,20 @@
       <c r="C116" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D116" s="9">
+      <c r="D116" s="29"/>
+      <c r="E116" s="9">
         <v>1</v>
       </c>
-      <c r="E116" s="9">
+      <c r="F116" s="9">
         <v>3</v>
       </c>
-      <c r="F116" s="9"/>
-      <c r="G116" s="12">
+      <c r="G116" s="9"/>
+      <c r="H116" s="12">
         <v>5000000</v>
       </c>
-      <c r="H116" s="9"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="9"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="30">
         <v>111</v>
       </c>
@@ -3715,19 +3927,20 @@
       <c r="C117" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D117" s="9">
+      <c r="D117" s="29"/>
+      <c r="E117" s="9">
         <v>1</v>
       </c>
-      <c r="E117" s="9">
+      <c r="F117" s="9">
         <v>5</v>
       </c>
-      <c r="F117" s="9"/>
-      <c r="G117" s="12">
+      <c r="G117" s="9"/>
+      <c r="H117" s="12">
         <v>3000000</v>
       </c>
-      <c r="H117" s="9"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="9"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="30">
         <v>112</v>
       </c>
@@ -3737,19 +3950,20 @@
       <c r="C118" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="D118" s="9" t="s">
+      <c r="D118" s="29"/>
+      <c r="E118" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E118" s="9" t="s">
+      <c r="F118" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F118" s="9"/>
-      <c r="G118" s="12">
+      <c r="G118" s="9"/>
+      <c r="H118" s="12">
         <v>1800000</v>
       </c>
-      <c r="H118" s="9"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="9"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="30">
         <v>113</v>
       </c>
@@ -3759,19 +3973,20 @@
       <c r="C119" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="D119" s="9" t="s">
+      <c r="D119" s="29"/>
+      <c r="E119" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E119" s="9" t="s">
+      <c r="F119" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F119" s="9"/>
-      <c r="G119" s="12">
+      <c r="G119" s="9"/>
+      <c r="H119" s="12">
         <v>2000000</v>
       </c>
-      <c r="H119" s="9"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="9"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="30">
         <v>114</v>
       </c>
@@ -3781,19 +3996,20 @@
       <c r="C120" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="D120" s="9" t="s">
+      <c r="D120" s="29"/>
+      <c r="E120" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="E120" s="9" t="s">
+      <c r="F120" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F120" s="9"/>
-      <c r="G120" s="12">
+      <c r="G120" s="9"/>
+      <c r="H120" s="12">
         <v>3000000</v>
       </c>
-      <c r="H120" s="9"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="9"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="30">
         <v>115</v>
       </c>
@@ -3803,19 +4019,20 @@
       <c r="C121" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="D121" s="9" t="s">
+      <c r="D121" s="29"/>
+      <c r="E121" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E121" s="9" t="s">
+      <c r="F121" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F121" s="9"/>
-      <c r="G121" s="12">
+      <c r="G121" s="9"/>
+      <c r="H121" s="12">
         <v>3000000</v>
       </c>
-      <c r="H121" s="9"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="9"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="30">
         <v>116</v>
       </c>
@@ -3825,19 +4042,20 @@
       <c r="C122" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="D122" s="9" t="s">
+      <c r="D122" s="29"/>
+      <c r="E122" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E122" s="9" t="s">
+      <c r="F122" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F122" s="9"/>
-      <c r="G122" s="12">
+      <c r="G122" s="9"/>
+      <c r="H122" s="12">
         <v>3000000</v>
       </c>
-      <c r="H122" s="9"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="9"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="30">
         <v>117</v>
       </c>
@@ -3847,70 +4065,71 @@
       <c r="C123" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="D123" s="9" t="s">
+      <c r="D123" s="29"/>
+      <c r="E123" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E123" s="9" t="s">
+      <c r="F123" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F123" s="9"/>
-      <c r="G123" s="12">
+      <c r="G123" s="9"/>
+      <c r="H123" s="12">
         <v>4000000</v>
       </c>
-      <c r="H123" s="9"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F127" s="34" t="s">
+      <c r="I123" s="9"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G127" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="G127" s="34"/>
-      <c r="H127" s="34"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F128" s="34" t="s">
+      <c r="H127" s="37"/>
+      <c r="I127" s="37"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G128" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="G128" s="34"/>
-      <c r="H128" s="34"/>
-    </row>
-    <row r="129" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F129" s="31"/>
+      <c r="H128" s="37"/>
+      <c r="I128" s="37"/>
+    </row>
+    <row r="129" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G129" s="31"/>
       <c r="H129" s="31"/>
-    </row>
-    <row r="130" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F130" s="32"/>
-      <c r="G130" s="31"/>
-      <c r="H130" s="32"/>
-    </row>
-    <row r="131" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F131" s="32"/>
-      <c r="G131" s="31"/>
-      <c r="H131" s="32"/>
-    </row>
-    <row r="132" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F132" s="33" t="s">
+      <c r="I129" s="31"/>
+    </row>
+    <row r="130" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G130" s="32"/>
+      <c r="H130" s="31"/>
+      <c r="I130" s="32"/>
+    </row>
+    <row r="131" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G131" s="32"/>
+      <c r="H131" s="31"/>
+      <c r="I131" s="32"/>
+    </row>
+    <row r="132" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G132" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="G132" s="33"/>
-      <c r="H132" s="33"/>
-    </row>
-    <row r="133" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F133" s="34" t="s">
+      <c r="H132" s="36"/>
+      <c r="I132" s="36"/>
+    </row>
+    <row r="133" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G133" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="G133" s="34"/>
-      <c r="H133" s="34"/>
+      <c r="H133" s="37"/>
+      <c r="I133" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="G132:I132"/>
+    <mergeCell ref="G133:I133"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A3:I3"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="G127:I127"/>
+    <mergeCell ref="G128:I128"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
@@ -3942,38 +4161,38 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -3986,11 +4205,11 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>

</xml_diff>

<commit_message>
edit DOKUMEN  PENDUKUNG/DATA DATA YANG HARUS DIMASUKAN/EKONOMI/RUMAH KOS DAN TOKO JAMU.xlsx
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/DATA DATA YANG HARUS DIMASUKAN/EKONOMI/RUMAH KOS DAN TOKO JAMU.xlsx
+++ b/DOKUMEN  PENDUKUNG/DATA DATA YANG HARUS DIMASUKAN/EKONOMI/RUMAH KOS DAN TOKO JAMU.xlsx
@@ -912,6 +912,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -927,11 +932,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1238,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="86" zoomScaleSheetLayoutView="86" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,41 +1256,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -1304,11 +1304,11 @@
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="33"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1339,7 +1339,7 @@
       <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="36" t="s">
         <v>195</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1368,7 +1368,7 @@
       <c r="C8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="37" t="s">
         <v>196</v>
       </c>
       <c r="E8" s="13">
@@ -1393,7 +1393,7 @@
       <c r="C9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="37" t="s">
         <v>196</v>
       </c>
       <c r="E9" s="13">
@@ -1639,7 +1639,7 @@
       <c r="C19" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E19" s="25">
@@ -1664,7 +1664,7 @@
       <c r="C20" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E20" s="13">
@@ -1689,7 +1689,7 @@
       <c r="C21" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E21" s="13">
@@ -1714,7 +1714,7 @@
       <c r="C22" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E22" s="13">
@@ -1739,7 +1739,7 @@
       <c r="C23" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="43" t="s">
+      <c r="D23" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E23" s="13">
@@ -1764,7 +1764,7 @@
       <c r="C24" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E24" s="13">
@@ -1789,7 +1789,7 @@
       <c r="C25" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E25" s="13">
@@ -1814,7 +1814,7 @@
       <c r="C26" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E26" s="13">
@@ -1839,7 +1839,7 @@
       <c r="C27" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E27" s="13">
@@ -1864,7 +1864,7 @@
       <c r="C28" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D28" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E28" s="13">
@@ -1889,7 +1889,7 @@
       <c r="C29" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E29" s="13">
@@ -1914,7 +1914,7 @@
       <c r="C30" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E30" s="13">
@@ -1939,7 +1939,7 @@
       <c r="C31" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="D31" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E31" s="13">
@@ -1964,7 +1964,7 @@
       <c r="C32" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="43" t="s">
+      <c r="D32" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E32" s="13">
@@ -1989,7 +1989,7 @@
       <c r="C33" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D33" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E33" s="13">
@@ -2014,7 +2014,7 @@
       <c r="C34" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D34" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E34" s="13">
@@ -2039,7 +2039,7 @@
       <c r="C35" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="43" t="s">
+      <c r="D35" s="38" t="s">
         <v>197</v>
       </c>
       <c r="E35" s="13">
@@ -4079,18 +4079,18 @@
       <c r="I123" s="9"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G127" s="37" t="s">
+      <c r="G127" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="H127" s="37"/>
-      <c r="I127" s="37"/>
+      <c r="H127" s="40"/>
+      <c r="I127" s="40"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G128" s="37" t="s">
+      <c r="G128" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="H128" s="37"/>
-      <c r="I128" s="37"/>
+      <c r="H128" s="40"/>
+      <c r="I128" s="40"/>
     </row>
     <row r="129" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G129" s="31"/>
@@ -4108,18 +4108,18 @@
       <c r="I131" s="32"/>
     </row>
     <row r="132" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G132" s="36" t="s">
+      <c r="G132" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="H132" s="36"/>
-      <c r="I132" s="36"/>
+      <c r="H132" s="39"/>
+      <c r="I132" s="39"/>
     </row>
     <row r="133" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G133" s="37" t="s">
+      <c r="G133" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="H133" s="37"/>
-      <c r="I133" s="37"/>
+      <c r="H133" s="40"/>
+      <c r="I133" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4161,38 +4161,38 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -4205,11 +4205,11 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>

</xml_diff>